<commit_message>
#Agregue la semana que faltaba con los valores actuales de las UATs.
</commit_message>
<xml_diff>
--- a/meetings/helpers/QC.20101018.xlsx
+++ b/meetings/helpers/QC.20101018.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Cobertura de la Prueba" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -136,7 +136,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES_tradnl"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -159,10 +159,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Cobertura de la Prueba'!$B$3:$B$12</c:f>
+              <c:f>'Cobertura de la Prueba'!$B$3:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -192,16 +192,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Cobertura de la Prueba'!$C$3:$C$12</c:f>
+              <c:f>'Cobertura de la Prueba'!$C$3:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -212,6 +215,9 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -234,10 +240,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Cobertura de la Prueba'!$B$3:$B$12</c:f>
+              <c:f>'Cobertura de la Prueba'!$B$3:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -267,16 +273,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Cobertura de la Prueba'!$D$3:$D$12</c:f>
+              <c:f>'Cobertura de la Prueba'!$D$3:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -288,6 +297,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -309,10 +321,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Cobertura de la Prueba'!$B$3:$B$12</c:f>
+              <c:f>'Cobertura de la Prueba'!$B$3:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -342,16 +354,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Cobertura de la Prueba'!$E$3:$E$12</c:f>
+              <c:f>'Cobertura de la Prueba'!$E$3:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -363,6 +378,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -384,10 +402,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Cobertura de la Prueba'!$B$3:$B$12</c:f>
+              <c:f>'Cobertura de la Prueba'!$B$3:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -417,16 +435,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Cobertura de la Prueba'!$F$3:$F$12</c:f>
+              <c:f>'Cobertura de la Prueba'!$F$3:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -438,17 +459,20 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="112377216"/>
-        <c:axId val="112379392"/>
+        <c:axId val="88611456"/>
+        <c:axId val="88622208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112377216"/>
+        <c:axId val="88611456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -460,7 +484,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr lang="en-US"/>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
@@ -474,14 +498,24 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112379392"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US"/>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="88622208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112379392"/>
+        <c:axId val="88622208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,7 +528,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr lang="en-US"/>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
@@ -508,7 +542,17 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112377216"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US"/>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="88611456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -516,17 +560,37 @@
         <c:showHorzBorder val="1"/>
         <c:showVertBorder val="1"/>
         <c:showOutline val="1"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr lang="en-US"/>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
       </c:dTable>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US"/>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -538,13 +602,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -568,8 +632,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:F12" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="A2:F12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:F13" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="A2:F13">
     <filterColumn colId="1"/>
   </autoFilter>
   <tableColumns count="6">
@@ -869,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -989,19 +1053,27 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="1">
-        <v>3</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="C7" s="1">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -1011,9 +1083,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="1">
-        <v>4</v>
-      </c>
+      <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -1023,19 +1093,19 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2">
+      <c r="A10" s="1">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>5</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="2">
         <v>9</v>
       </c>
@@ -1045,7 +1115,9 @@
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2">
+        <v>5</v>
+      </c>
       <c r="B12" s="2">
         <v>10</v>
       </c>
@@ -1053,6 +1125,16 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>